<commit_message>
update reference corrections data
</commit_message>
<xml_diff>
--- a/refCorrections.xlsx
+++ b/refCorrections.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rfiorella/Documents/NEONiso-LANL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48C4BC-4EFA-1944-AA7B-530A038F25C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA98678-AE0F-A446-827B-178A20B6FDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="500" windowWidth="23140" windowHeight="27160" xr2:uid="{373B1C11-4CB9-2A4C-B768-574E997643BF}"/>
+    <workbookView xWindow="13480" yWindow="500" windowWidth="23140" windowHeight="27160" xr2:uid="{373B1C11-4CB9-2A4C-B768-574E997643BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>site</t>
   </si>
@@ -110,9 +110,6 @@
   </si>
   <si>
     <t>MOAB</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>notes</t>
@@ -499,7 +496,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +525,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -537,13 +534,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -562,18 +559,14 @@
       <c r="E2" s="4">
         <v>509.34</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="4"/>
       <c r="G2" t="b">
         <v>0</v>
       </c>
       <c r="H2" s="4">
         <v>-9.6530000000000005</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="I2" s="6"/>
       <c r="J2" t="b">
         <v>0</v>
       </c>
@@ -597,18 +590,14 @@
       <c r="E3" s="4">
         <v>508.42</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F3" s="4"/>
       <c r="G3" t="b">
         <v>0</v>
       </c>
       <c r="H3" s="4">
         <v>-9.2650000000000006</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="I3" s="6"/>
       <c r="J3" t="b">
         <v>0</v>
       </c>
@@ -632,18 +621,14 @@
       <c r="E4" s="4">
         <v>532.79999999999995</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F4" s="4"/>
       <c r="G4" t="b">
         <v>0</v>
       </c>
       <c r="H4" s="4">
         <v>-13.038</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="I4" s="6"/>
       <c r="J4" t="b">
         <v>0</v>
       </c>
@@ -667,18 +652,14 @@
       <c r="E5" s="4">
         <v>525.05999999999995</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F5" s="4"/>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="H5" s="4">
         <v>-10.391</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="I5" s="6"/>
       <c r="J5" t="b">
         <v>0</v>
       </c>
@@ -702,18 +683,14 @@
       <c r="E6" s="4">
         <v>506.98</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" t="b">
         <v>0</v>
       </c>
       <c r="H6" s="4">
         <v>-9.5347000000000008</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="I6" s="6"/>
       <c r="J6" t="b">
         <v>0</v>
       </c>
@@ -737,18 +714,14 @@
       <c r="E7" s="4">
         <v>367.88</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F7" s="4"/>
       <c r="G7" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="4">
         <v>-12.372</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="I7" s="6"/>
       <c r="J7" t="b">
         <v>0</v>
       </c>
@@ -772,18 +745,14 @@
       <c r="E8" s="4">
         <v>444.1</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="F8" s="4"/>
       <c r="G8" t="b">
         <v>0</v>
       </c>
       <c r="H8" s="4">
         <v>-9.0549999999999997</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="I8" s="6"/>
       <c r="J8" t="b">
         <v>0</v>
       </c>
@@ -1141,7 +1110,7 @@
         <v>0.6</v>
       </c>
       <c r="L18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1179,7 +1148,7 @@
         <v>0.6</v>
       </c>
       <c r="L19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>